<commit_message>
Update metadata in the sites
Update metadata in the sites
</commit_message>
<xml_diff>
--- a/data/list_sites.xlsx
+++ b/data/list_sites.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fuentesm\Marilu\Deltares\Projects\AGAME\GitHub\vlabs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C29CFE71-974A-42A2-8D88-C1D91D763C4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6FE3994-41C3-451A-B3D8-0B0F78ACA640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="1440" windowWidth="17280" windowHeight="9030" xr2:uid="{09AA9583-AA21-4EED-89F0-A10E405DEC63}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09AA9583-AA21-4EED-89F0-A10E405DEC63}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>site name</t>
   </si>
@@ -114,6 +114,27 @@
   </si>
   <si>
     <t>evergreen needleleaf forests</t>
+  </si>
+  <si>
+    <t>https://meta.icos-cp.eu/resources/stations/ES_IT-Tor</t>
+  </si>
+  <si>
+    <t>Metadata</t>
+  </si>
+  <si>
+    <t>https://www.icos-belgium.be/ESLonzee.php</t>
+  </si>
+  <si>
+    <t>https://meta.icos-cp.eu/resources/stations/ES_BE-Lon</t>
+  </si>
+  <si>
+    <t>https://meta.icos-cp.eu/resources/stations/ES_DE-HoH</t>
+  </si>
+  <si>
+    <t>canopy</t>
+  </si>
+  <si>
+    <t>instrument</t>
   </si>
 </sst>
 </file>
@@ -465,24 +486,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB49A176-4204-4AFA-A3DF-E3F4EAE4A3B9}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -504,8 +526,17 @@
       <c r="G1" t="s">
         <v>7</v>
       </c>
+      <c r="H1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -528,7 +559,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -550,8 +581,14 @@
       <c r="G3">
         <v>170</v>
       </c>
+      <c r="J3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -573,8 +610,17 @@
       <c r="G4">
         <v>193</v>
       </c>
+      <c r="H4">
+        <v>45</v>
+      </c>
+      <c r="I4">
+        <v>33</v>
+      </c>
+      <c r="J4" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -596,8 +642,11 @@
       <c r="G5">
         <v>2168</v>
       </c>
+      <c r="J5" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Canopy height and instrument height for France site
Canopy height and instrument height for France site
</commit_message>
<xml_diff>
--- a/data/list_sites.xlsx
+++ b/data/list_sites.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fuentesm\Marilu\Deltares\Projects\AGAME\GitHub\vlabs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6FE3994-41C3-451A-B3D8-0B0F78ACA640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41CC777E-901C-45C3-AEFA-C5A3EE513332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09AA9583-AA21-4EED-89F0-A10E405DEC63}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>site name</t>
   </si>
@@ -135,16 +135,27 @@
   </si>
   <si>
     <t>instrument</t>
+  </si>
+  <si>
+    <t>https://meta.icos-cp.eu/resources/stations/ES_FR-EM2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -167,13 +178,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -489,7 +503,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,6 +572,15 @@
       <c r="G2">
         <v>85</v>
       </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>0.7</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -670,7 +693,10 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{B81F5B6F-B155-43AD-8226-D8114333511C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update time series processing
Update time series processing
</commit_message>
<xml_diff>
--- a/data/list_sites.xlsx
+++ b/data/list_sites.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fuentesm\Marilu\Deltares\Projects\AGAME\GitHub\vlabs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41CC777E-901C-45C3-AEFA-C5A3EE513332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{018651AD-645C-4418-85B6-D1303C304B01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09AA9583-AA21-4EED-89F0-A10E405DEC63}"/>
   </bookViews>
@@ -503,7 +503,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Revert "Update time series processing"
This reverts commit eedf6a8990ac2fc9c23a45b0c66ede97fb498400.
</commit_message>
<xml_diff>
--- a/data/list_sites.xlsx
+++ b/data/list_sites.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fuentesm\Marilu\Deltares\Projects\AGAME\GitHub\vlabs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{018651AD-645C-4418-85B6-D1303C304B01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41CC777E-901C-45C3-AEFA-C5A3EE513332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09AA9583-AA21-4EED-89F0-A10E405DEC63}"/>
   </bookViews>
@@ -503,7 +503,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>